<commit_message>
Lab 4 part 3 was edited with teacher's requriments
</commit_message>
<xml_diff>
--- a/LABS/lab04/part3/result.xlsx
+++ b/LABS/lab04/part3/result.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
@@ -596,13 +596,23 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="4" t="inlineStr">
         <is>
           <t>Телевизор</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" s="4" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Стиральная машина</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>